<commit_message>
Quitar datos vacios correspondientes, cambiarescolaridad a años, graficar de nuevo con los datos filtrados
</commit_message>
<xml_diff>
--- a/Calendario de actividades.xlsx
+++ b/Calendario de actividades.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\valec\Documents\JI\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\valec\Documents\JI\Codigos\Data_analysis_ML_Harmonization_Proyect\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9F622A5-31CD-4656-8609-CA3F03CA9646}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C64D427A-4794-49D1-8F22-351A7E12BEEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="696" yWindow="1620" windowWidth="17280" windowHeight="10620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Actividades durante la pasantia" sheetId="1" r:id="rId1"/>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="92">
   <si>
     <t>Fecha</t>
   </si>
@@ -343,6 +343,9 @@
   </si>
   <si>
     <t>Pruebas suiza y comenzar curso de agenda cientifica de manejo de datos con herramientas de google</t>
+  </si>
+  <si>
+    <t>Curso de manejo de datos con herramientas de google,  nuevo dataframe sin datos vacios, graficos (solo componentes esto) y cambio de escolaridad por años</t>
   </si>
 </sst>
 </file>
@@ -838,10 +841,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D73"/>
+  <dimension ref="A1:D74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C73" sqref="C73"/>
+    <sheetView tabSelected="1" topLeftCell="A68" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C74" sqref="C74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1687,7 +1690,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="73" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:3" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A73" s="18">
         <v>44726</v>
       </c>
@@ -1696,6 +1699,17 @@
       </c>
       <c r="C73" s="9">
         <v>7</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" ht="55.2" x14ac:dyDescent="0.3">
+      <c r="A74" s="18">
+        <v>44761</v>
+      </c>
+      <c r="B74" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="C74" s="9">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Corrección de la cantidad de datos vacios y corrección del filtrado, Pendiente: pruebas estadisticas y BIOMARCADORES CON TODOS LOS DATOS
</commit_message>
<xml_diff>
--- a/Calendario de actividades.xlsx
+++ b/Calendario de actividades.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\valec\Documents\JI\Codigos\Data_analysis_ML_Harmonization_Proyect\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C64D427A-4794-49D1-8F22-351A7E12BEEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{786ABC35-579E-4CF1-9DC4-006837782621}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="696" yWindow="1620" windowWidth="17280" windowHeight="10620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Actividades durante la pasantia" sheetId="1" r:id="rId1"/>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="95">
   <si>
     <t>Fecha</t>
   </si>
@@ -346,6 +346,15 @@
   </si>
   <si>
     <t>Curso de manejo de datos con herramientas de google,  nuevo dataframe sin datos vacios, graficos (solo componentes esto) y cambio de escolaridad por años</t>
+  </si>
+  <si>
+    <t>Curso de manejo de datos</t>
+  </si>
+  <si>
+    <t>23(07/2022</t>
+  </si>
+  <si>
+    <t>Reunion con vero organizando el codigo con datos vacios</t>
   </si>
 </sst>
 </file>
@@ -841,10 +850,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D74"/>
+  <dimension ref="A1:D76"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A68" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C74" sqref="C74"/>
+      <selection activeCell="C76" sqref="C76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1709,7 +1718,29 @@
         <v>91</v>
       </c>
       <c r="C74" s="9">
-        <v>5</v>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A75" s="18">
+        <v>44763</v>
+      </c>
+      <c r="B75" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="C75" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A76" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B76" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C76" s="9">
+        <v>1.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
graficos ICC con bandas en x y barras de error
</commit_message>
<xml_diff>
--- a/Calendario de actividades.xlsx
+++ b/Calendario de actividades.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\valec\Documents\JI\Codigos\Data_analysis_ML_Harmonization_Proyect\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{786ABC35-579E-4CF1-9DC4-006837782621}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F23062E-CA8D-490D-8F14-F2ABE70F242E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="102">
   <si>
     <t>Fecha</t>
   </si>
@@ -351,10 +351,31 @@
     <t>Curso de manejo de datos</t>
   </si>
   <si>
-    <t>23(07/2022</t>
-  </si>
-  <si>
     <t>Reunion con vero organizando el codigo con datos vacios</t>
+  </si>
+  <si>
+    <t>Apoyo pruebas suiza, curso manejo de datos, reunion con vero del articulo</t>
+  </si>
+  <si>
+    <t>Reunion con vero y luisa, curso manejo de datos</t>
+  </si>
+  <si>
+    <t>curso manejo de datos</t>
+  </si>
+  <si>
+    <t>Revision articulos reactividad</t>
+  </si>
+  <si>
+    <t>Reunion con vero y luisa reactividad, curso manejo de datos</t>
+  </si>
+  <si>
+    <t>Parque explora apropiacion social del conocimiento</t>
+  </si>
+  <si>
+    <t>Finalizacion del curso de manejo de datos con herramientas de googles</t>
+  </si>
+  <si>
+    <t>Graficos ICC solo por bandas</t>
   </si>
 </sst>
 </file>
@@ -850,10 +871,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D76"/>
+  <dimension ref="A1:D84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A68" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C76" sqref="C76"/>
+    <sheetView tabSelected="1" topLeftCell="A73" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C84" sqref="C84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -880,7 +901,7 @@
     </row>
     <row r="2" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="19" cm="1">
-        <f t="array" aca="1" ref="A2" ca="1">A2:A2929/10/2021</f>
+        <f t="array" aca="1" ref="A2" ca="1">A2:A2930/10/2021</f>
         <v>0</v>
       </c>
       <c r="B2" s="12" t="s">
@@ -1733,14 +1754,102 @@
       </c>
     </row>
     <row r="76" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A76" s="2" t="s">
+      <c r="A76" s="18">
+        <v>44765</v>
+      </c>
+      <c r="B76" s="2" t="s">
         <v>93</v>
-      </c>
-      <c r="B76" s="2" t="s">
-        <v>94</v>
       </c>
       <c r="C76" s="9">
         <v>1.5</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A77" s="18">
+        <v>44768</v>
+      </c>
+      <c r="B77" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C77" s="9">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A78" s="18">
+        <v>44775</v>
+      </c>
+      <c r="B78" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C78" s="9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A79" s="18">
+        <v>44777</v>
+      </c>
+      <c r="B79" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C79" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A80" s="18">
+        <v>44780</v>
+      </c>
+      <c r="B80" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C80" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A81" s="18">
+        <v>44782</v>
+      </c>
+      <c r="B81" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="C81" s="9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A82" s="18">
+        <v>44783</v>
+      </c>
+      <c r="B82" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="C82" s="9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A83" s="18">
+        <v>44784</v>
+      </c>
+      <c r="B83" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="C83" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A84" s="18">
+        <v>44789</v>
+      </c>
+      <c r="B84" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C84" s="9">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualizacion de graficos ICC y test de diferencia entre grupos evaluado por cada banda de frecuencia
</commit_message>
<xml_diff>
--- a/Calendario de actividades.xlsx
+++ b/Calendario de actividades.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\valec\Documents\JI\Codigos\Data_analysis_ML_Harmonization_Proyect\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F23062E-CA8D-490D-8F14-F2ABE70F242E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9EE14E7-8A71-4768-BDC3-B83A31E69C3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="107">
   <si>
     <t>Fecha</t>
   </si>
@@ -375,7 +375,22 @@
     <t>Finalizacion del curso de manejo de datos con herramientas de googles</t>
   </si>
   <si>
-    <t>Graficos ICC solo por bandas</t>
+    <t>Graficos ICC solo por bandas, pruebas estadisticas, normalidad y ANOVA no parametrico implementado a los ICC de CTR y G2</t>
+  </si>
+  <si>
+    <t>Reunion de avances</t>
+  </si>
+  <si>
+    <t>Reunion luisa Staff</t>
+  </si>
+  <si>
+    <t>preparacion staff</t>
+  </si>
+  <si>
+    <t>Presentacion staff</t>
+  </si>
+  <si>
+    <t>Reunión ASC</t>
   </si>
 </sst>
 </file>
@@ -871,10 +886,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D84"/>
+  <dimension ref="A1:D89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C84" sqref="C84"/>
+    <sheetView tabSelected="1" topLeftCell="A75" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C87" sqref="C87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1841,7 +1856,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:3" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A84" s="18">
         <v>44789</v>
       </c>
@@ -1849,7 +1864,62 @@
         <v>101</v>
       </c>
       <c r="C84" s="9">
-        <v>2</v>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A85" s="18">
+        <v>44791</v>
+      </c>
+      <c r="B85" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="C85" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A86" s="18">
+        <v>44792</v>
+      </c>
+      <c r="B86" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="C86" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A87" s="18">
+        <v>44794</v>
+      </c>
+      <c r="B87" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="C87" s="9">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A88" s="18">
+        <v>44795</v>
+      </c>
+      <c r="B88" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="C88" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A89" s="18">
+        <v>44795</v>
+      </c>
+      <c r="B89" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="C89" s="9">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Información de las bases de datos organizados y prueba de normalidad aplicada a las componentes
</commit_message>
<xml_diff>
--- a/Calendario de actividades.xlsx
+++ b/Calendario de actividades.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\valec\Documents\JI\Codigos\Data_analysis_ML_Harmonization_Proyect\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8745FAA6-5E80-4175-9EDC-79A3FC4C7EDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0A51BB3-B121-4F91-A279-8C0D88F915F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="110">
   <si>
     <t>Fecha</t>
   </si>
@@ -397,6 +397,9 @@
   </si>
   <si>
     <t>Reuinion de revision de biomarcadores</t>
+  </si>
+  <si>
+    <t>Organizar datos de las bases de datos</t>
   </si>
 </sst>
 </file>
@@ -892,10 +895,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D91"/>
+  <dimension ref="A1:D92"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A81" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C91" sqref="C91"/>
+      <selection activeCell="C92" sqref="C92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1948,6 +1951,17 @@
       </c>
       <c r="C91" s="9">
         <v>3</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A92" s="18">
+        <v>44803</v>
+      </c>
+      <c r="B92" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C92" s="9">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Nuevos resultados de diferencias grupales de ICC por IC y Rois
</commit_message>
<xml_diff>
--- a/Calendario de actividades.xlsx
+++ b/Calendario de actividades.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\valec\Documents\JI\Codigos\Data_analysis_ML_Harmonization_Proyect\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0A51BB3-B121-4F91-A279-8C0D88F915F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E38D8EE-C493-4FA6-91CC-A98FFD8C4EA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="111">
   <si>
     <t>Fecha</t>
   </si>
@@ -400,6 +400,9 @@
   </si>
   <si>
     <t>Organizar datos de las bases de datos</t>
+  </si>
+  <si>
+    <t>Reunion con xime articulo ICC, calculo d enuevos resultados y obtencion de informacion demografica</t>
   </si>
 </sst>
 </file>
@@ -895,10 +898,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D92"/>
+  <dimension ref="A1:D93"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A81" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C92" sqref="C92"/>
+      <selection activeCell="C93" sqref="C93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1962,6 +1965,17 @@
       </c>
       <c r="C92" s="9">
         <v>9</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A93" s="18">
+        <v>44774</v>
+      </c>
+      <c r="B93" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="C93" s="9">
+        <v>2.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Convertir los datos por columnas a un formato largo para hacer los graficos
</commit_message>
<xml_diff>
--- a/Calendario de actividades.xlsx
+++ b/Calendario de actividades.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\valec\Documents\JI\Codigos\Data_analysis_ML_Harmonization_Proyect\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E38D8EE-C493-4FA6-91CC-A98FFD8C4EA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D626DC74-2394-4AEF-A6CB-E0A78EC06586}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="113">
   <si>
     <t>Fecha</t>
   </si>
@@ -403,6 +403,12 @@
   </si>
   <si>
     <t>Reunion con xime articulo ICC, calculo d enuevos resultados y obtencion de informacion demografica</t>
+  </si>
+  <si>
+    <t>3(08/2022</t>
+  </si>
+  <si>
+    <t>Reunion con alberto de normalización, donde recomendo el empezar a usar combat</t>
   </si>
 </sst>
 </file>
@@ -898,10 +904,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D93"/>
+  <dimension ref="A1:D94"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A81" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C93" sqref="C93"/>
+      <selection activeCell="C94" sqref="C94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1975,7 +1981,18 @@
         <v>110</v>
       </c>
       <c r="C93" s="9">
-        <v>2.5</v>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A94" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="B94" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="C94" s="9">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Union base de datos DUQUE al dataframe y graficos
</commit_message>
<xml_diff>
--- a/Calendario de actividades.xlsx
+++ b/Calendario de actividades.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\valec\Documents\JI\Codigos\Data_analysis_ML_Harmonization_Proyect\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF46C2DB-DE2D-43D3-9620-D2C98B274EAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76A611E0-D185-453B-8281-027270280777}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="117">
   <si>
     <t>Fecha</t>
   </si>
@@ -412,6 +412,15 @@
   </si>
   <si>
     <t xml:space="preserve">Crear nuevo dataframe para los datos de biomarcadores </t>
+  </si>
+  <si>
+    <t>Nuevos graficos articulo ICC, lectura de articulo profe mando</t>
+  </si>
+  <si>
+    <t>Cedulas de la base de datos de duque, asesoria de ASC con los estudiantes.</t>
+  </si>
+  <si>
+    <t>Reunion con vero, lectura de articulos</t>
   </si>
 </sst>
 </file>
@@ -907,10 +916,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D96"/>
+  <dimension ref="A1:D99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C96" sqref="C96"/>
+    <sheetView tabSelected="1" topLeftCell="A88" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C99" sqref="C99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2018,6 +2027,39 @@
       </c>
       <c r="C96" s="9">
         <v>3</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A97" s="18">
+        <v>44786</v>
+      </c>
+      <c r="B97" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="C97" s="9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A98" s="18">
+        <v>44788</v>
+      </c>
+      <c r="B98" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="C98" s="9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A99" s="18">
+        <v>44793</v>
+      </c>
+      <c r="B99" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="C99" s="9">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
"graficos para datos demograficos, dataframe y graficos con los grupos DB de DUQUE"
</commit_message>
<xml_diff>
--- a/Calendario de actividades.xlsx
+++ b/Calendario de actividades.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\valec\Documents\JI\Codigos\Data_analysis_ML_Harmonization_Proyect\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76A611E0-D185-453B-8281-027270280777}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40808A4A-CF9C-4E98-825A-AC9FF4A4632D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -919,7 +919,7 @@
   <dimension ref="A1:D99"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A88" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C99" sqref="C99"/>
+      <selection activeCell="D101" sqref="D101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2059,7 +2059,7 @@
         <v>116</v>
       </c>
       <c r="C99" s="9">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
"Actualizacion de actividades realizadas"
</commit_message>
<xml_diff>
--- a/Calendario de actividades.xlsx
+++ b/Calendario de actividades.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\valec\Documents\JI\Codigos\Data_analysis_ML_Harmonization_Proyect\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40808A4A-CF9C-4E98-825A-AC9FF4A4632D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A84AB3E-84F7-428D-9660-78FD3373A72C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="119">
   <si>
     <t>Fecha</t>
   </si>
@@ -421,6 +421,12 @@
   </si>
   <si>
     <t>Reunion con vero, lectura de articulos</t>
+  </si>
+  <si>
+    <t>Ver genero de la base de datos de duque</t>
+  </si>
+  <si>
+    <t>Graficos de distribucion de los datos demograficos, organizar las graficas de nuevo con los grupos de la base de datos de duque, reunion de avances con el profe</t>
   </si>
 </sst>
 </file>
@@ -916,10 +922,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D99"/>
+  <dimension ref="A1:D101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A88" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D101" sqref="D101"/>
+    <sheetView tabSelected="1" topLeftCell="A89" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="D100" sqref="D100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2060,6 +2066,28 @@
       </c>
       <c r="C99" s="9">
         <v>7</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" ht="55.2" x14ac:dyDescent="0.3">
+      <c r="A100" s="18">
+        <v>44795</v>
+      </c>
+      <c r="B100" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="C100" s="9">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A101" s="18">
+        <v>44796</v>
+      </c>
+      <c r="B101" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="C101" s="9">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
"Resultados de las pruebas estadisticas de diferencias grupales en un archivo csv"
</commit_message>
<xml_diff>
--- a/Calendario de actividades.xlsx
+++ b/Calendario de actividades.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\valec\Documents\JI\Codigos\Data_analysis_ML_Harmonization_Proyect\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A84AB3E-84F7-428D-9660-78FD3373A72C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53959880-6500-4685-B73C-C69A1CBE0A61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2436" yWindow="1620" windowWidth="17280" windowHeight="10620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Actividades durante la pasantia" sheetId="1" r:id="rId1"/>
@@ -924,8 +924,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A89" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D100" sqref="D100"/>
+    <sheetView tabSelected="1" topLeftCell="A93" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C100" sqref="C100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2076,7 +2076,7 @@
         <v>118</v>
       </c>
       <c r="C100" s="9">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
"Actualizacion de todo al añadir genero de la DB DUQUE"
</commit_message>
<xml_diff>
--- a/Calendario de actividades.xlsx
+++ b/Calendario de actividades.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\valec\Documents\JI\Codigos\Data_analysis_ML_Harmonization_Proyect\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53959880-6500-4685-B73C-C69A1CBE0A61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3564E7A-8708-4629-A5AE-6AC5814CD962}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2436" yWindow="1620" windowWidth="17280" windowHeight="10620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -423,10 +423,10 @@
     <t>Reunion con vero, lectura de articulos</t>
   </si>
   <si>
-    <t>Ver genero de la base de datos de duque</t>
-  </si>
-  <si>
     <t>Graficos de distribucion de los datos demograficos, organizar las graficas de nuevo con los grupos de la base de datos de duque, reunion de avances con el profe</t>
+  </si>
+  <si>
+    <t>Ver genero de la base de datos de duque y actualizar codigos con esto y graficos</t>
   </si>
 </sst>
 </file>
@@ -925,7 +925,7 @@
   <dimension ref="A1:D101"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A93" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C100" sqref="C100"/>
+      <selection activeCell="B101" sqref="B101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2073,21 +2073,21 @@
         <v>44795</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C100" s="9">
         <v>10</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A101" s="18">
         <v>44796</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C101" s="9">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
"Codigo nuevo de datos atipicos por IC"
</commit_message>
<xml_diff>
--- a/Calendario de actividades.xlsx
+++ b/Calendario de actividades.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\valec\Documents\JI\Codigos\Data_analysis_ML_Harmonization_Proyect\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3564E7A-8708-4629-A5AE-6AC5814CD962}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{635D6AD0-D0E4-4212-9007-38EA55188EC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2436" yWindow="1620" windowWidth="17280" windowHeight="10620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Actividades durante la pasantia" sheetId="1" r:id="rId1"/>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="120">
   <si>
     <t>Fecha</t>
   </si>
@@ -427,6 +427,9 @@
   </si>
   <si>
     <t>Ver genero de la base de datos de duque y actualizar codigos con esto y graficos</t>
+  </si>
+  <si>
+    <t>Revision de datos atipicos componentes</t>
   </si>
 </sst>
 </file>
@@ -922,10 +925,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D101"/>
+  <dimension ref="A1:D103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A93" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B101" sqref="B101"/>
+    <sheetView tabSelected="1" topLeftCell="A89" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B103" sqref="B103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1993,7 +1996,7 @@
     </row>
     <row r="93" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A93" s="18">
-        <v>44774</v>
+        <v>44805</v>
       </c>
       <c r="B93" s="2" t="s">
         <v>110</v>
@@ -2004,7 +2007,7 @@
     </row>
     <row r="94" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A94" s="18">
-        <v>44776</v>
+        <v>44807</v>
       </c>
       <c r="B94" s="2" t="s">
         <v>111</v>
@@ -2015,7 +2018,7 @@
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A95" s="18">
-        <v>44779</v>
+        <v>44810</v>
       </c>
       <c r="B95" s="2" t="s">
         <v>112</v>
@@ -2026,7 +2029,7 @@
     </row>
     <row r="96" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A96" s="18">
-        <v>44781</v>
+        <v>44812</v>
       </c>
       <c r="B96" s="2" t="s">
         <v>113</v>
@@ -2037,7 +2040,7 @@
     </row>
     <row r="97" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A97" s="18">
-        <v>44786</v>
+        <v>44817</v>
       </c>
       <c r="B97" s="2" t="s">
         <v>114</v>
@@ -2048,7 +2051,7 @@
     </row>
     <row r="98" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A98" s="18">
-        <v>44788</v>
+        <v>44819</v>
       </c>
       <c r="B98" s="2" t="s">
         <v>115</v>
@@ -2059,7 +2062,7 @@
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A99" s="18">
-        <v>44793</v>
+        <v>44824</v>
       </c>
       <c r="B99" s="2" t="s">
         <v>116</v>
@@ -2070,7 +2073,7 @@
     </row>
     <row r="100" spans="1:3" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A100" s="18">
-        <v>44795</v>
+        <v>44826</v>
       </c>
       <c r="B100" s="2" t="s">
         <v>117</v>
@@ -2087,6 +2090,28 @@
         <v>118</v>
       </c>
       <c r="C101" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A102" s="18">
+        <v>44833</v>
+      </c>
+      <c r="B102" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C102" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A103" s="18">
+        <v>44839</v>
+      </c>
+      <c r="B103" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="C103" s="9">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
"Eliminacion de datos atipicos y graficos (IC-ROI)"
</commit_message>
<xml_diff>
--- a/Calendario de actividades.xlsx
+++ b/Calendario de actividades.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\valec\Documents\JI\Codigos\Data_analysis_ML_Harmonization_Proyect\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{635D6AD0-D0E4-4212-9007-38EA55188EC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{384704B7-DDD8-438E-BC7F-B4DFC6DD9169}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="122">
   <si>
     <t>Fecha</t>
   </si>
@@ -430,6 +430,12 @@
   </si>
   <si>
     <t>Revision de datos atipicos componentes</t>
+  </si>
+  <si>
+    <t>Asesoria ASC retos explora</t>
+  </si>
+  <si>
+    <t>Eliminacion de datos atipicos de Rois y graficos, revision articulo, reunion carlos.</t>
   </si>
 </sst>
 </file>
@@ -925,10 +931,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D103"/>
+  <dimension ref="A1:D105"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A89" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B103" sqref="B103"/>
+    <sheetView tabSelected="1" topLeftCell="A97" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C105" sqref="C105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2113,6 +2119,28 @@
       </c>
       <c r="C103" s="9">
         <v>2</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A104" s="18">
+        <v>44840</v>
+      </c>
+      <c r="B104" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="C104" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A105" s="18">
+        <v>44841</v>
+      </c>
+      <c r="B105" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="C105" s="9">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
sl y coherencia obtener dataframes
</commit_message>
<xml_diff>
--- a/Calendario de actividades.xlsx
+++ b/Calendario de actividades.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\valec\Documents\JI\Codigos\Data_analysis_ML_Harmonization_Proyect\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{384704B7-DDD8-438E-BC7F-B4DFC6DD9169}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF526F60-F367-47F7-A6A0-A6B65E78EC2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="127">
   <si>
     <t>Fecha</t>
   </si>
@@ -436,6 +436,21 @@
   </si>
   <si>
     <t>Eliminacion de datos atipicos de Rois y graficos, revision articulo, reunion carlos.</t>
+  </si>
+  <si>
+    <t>Discusion articulo</t>
+  </si>
+  <si>
+    <t>Busqueda de articulos</t>
+  </si>
+  <si>
+    <t>Busqueda de articulos ASC, reunion vero</t>
+  </si>
+  <si>
+    <t>Revision huber con vero, articulos y preguntas ASC para los retos explora</t>
+  </si>
+  <si>
+    <t>Obtener dataframes por columnas de SL, coherencia</t>
   </si>
 </sst>
 </file>
@@ -931,10 +946,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D105"/>
+  <dimension ref="A1:D111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A97" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C105" sqref="C105"/>
+    <sheetView tabSelected="1" topLeftCell="A101" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C111" sqref="C111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -961,7 +976,7 @@
     </row>
     <row r="2" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="19" cm="1">
-        <f t="array" aca="1" ref="A2" ca="1">A2:A2930/10/2021</f>
+        <f t="array" aca="1" ref="A2" ca="1">A2:A2931/10/2021</f>
         <v>0</v>
       </c>
       <c r="B2" s="12" t="s">
@@ -2141,6 +2156,72 @@
       </c>
       <c r="C105" s="9">
         <v>4</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A106" s="18">
+        <v>44843</v>
+      </c>
+      <c r="B106" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="C106" s="9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A107" s="18">
+        <v>44844</v>
+      </c>
+      <c r="B107" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="C107" s="9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A108" s="18">
+        <v>44845</v>
+      </c>
+      <c r="B108" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="C108" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A109" s="18">
+        <v>44846</v>
+      </c>
+      <c r="B109" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="C109" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A110" s="18">
+        <v>44849</v>
+      </c>
+      <c r="B110" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="C110" s="9">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A111" s="18">
+        <v>44852</v>
+      </c>
+      <c r="B111" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="C111" s="9">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Union dataframes con SL y coherencia, graficos
</commit_message>
<xml_diff>
--- a/Calendario de actividades.xlsx
+++ b/Calendario de actividades.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\valec\Documents\JI\Codigos\Data_analysis_ML_Harmonization_Proyect\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF526F60-F367-47F7-A6A0-A6B65E78EC2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6B1BCF8-376A-4636-ADED-1A44E6ECE893}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="128">
   <si>
     <t>Fecha</t>
   </si>
@@ -451,6 +451,9 @@
   </si>
   <si>
     <t>Obtener dataframes por columnas de SL, coherencia</t>
+  </si>
+  <si>
+    <t>Articulos vision, dataframes con SL y coherencia, y codigo para graficos</t>
   </si>
 </sst>
 </file>
@@ -946,10 +949,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D111"/>
+  <dimension ref="A1:D112"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A101" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C111" sqref="C111"/>
+      <selection activeCell="C112" sqref="C112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2222,6 +2225,17 @@
       </c>
       <c r="C111" s="9">
         <v>8</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A112" s="18">
+        <v>44853</v>
+      </c>
+      <c r="B112" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="C112" s="9">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
tablas edad,educacion y genero por DB
</commit_message>
<xml_diff>
--- a/Calendario de actividades.xlsx
+++ b/Calendario de actividades.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\valec\Documents\JI\Codigos\Data_analysis_ML_Harmonization_Proyect\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6B1BCF8-376A-4636-ADED-1A44E6ECE893}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DC9477A-883C-4260-8440-AF2CEE609D6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="130">
   <si>
     <t>Fecha</t>
   </si>
@@ -454,6 +454,12 @@
   </si>
   <si>
     <t>Articulos vision, dataframes con SL y coherencia, y codigo para graficos</t>
+  </si>
+  <si>
+    <t>Tablas de edad, educion y sexo por bases de datos</t>
+  </si>
+  <si>
+    <t>Ear dream y reunion con emilse</t>
   </si>
 </sst>
 </file>
@@ -949,10 +955,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D112"/>
+  <dimension ref="A1:D114"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A101" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C112" sqref="C112"/>
+      <selection activeCell="C114" sqref="C114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2235,7 +2241,29 @@
         <v>127</v>
       </c>
       <c r="C112" s="9">
-        <v>6</v>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A113" s="18">
+        <v>44854</v>
+      </c>
+      <c r="B113" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C113" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A114" s="18">
+        <v>44855</v>
+      </c>
+      <c r="B114" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C114" s="9">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>